<commit_message>
First product with with complete-ish costing tables for three diseases and their sequelae
All cost items for three diseases (Salmonella, Campy, and Shigella) together with their sequelae. However there are some missing cost elements (e.g. some WTP and human capital costs for sequelae) and some some cost items (e.g. some medications to be finalised). The interactive table allows comparisons of all cost times for all diseases and agegroups
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7B8337-6EDE-2649-99C7-AD58FED3EFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E224FF-C252-2849-87D0-67846A26A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12740" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18280" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>Cost</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Weighted sum of MCS (69345) and PCR (69496). Following Ford2019 we used weights: 0.91 and .55. Weights don't add to 1 because 46% of people are thought to have both sets of tests</t>
+  </si>
+  <si>
+    <t>B06A</t>
   </si>
 </sst>
 </file>
@@ -1103,15 +1106,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="13.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1614,6 +1617,17 @@
         <v>58</v>
       </c>
     </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2">
+        <v>28927</v>
+      </c>
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement 'All Gastro', Toxo and Typhoid.
Also nearly completed Listeria, but need to fix how the program handles the case when there are no hospitalisations for a given age-group for a given year before Listeria can be exposed
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E224FF-C252-2849-87D0-67846A26A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831A39F8-5AD7-6847-A608-C95C1A053C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18280" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="460" windowWidth="18280" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
   <si>
     <t>Cost</t>
   </si>
@@ -244,6 +244,33 @@
   </si>
   <si>
     <t>B06A</t>
+  </si>
+  <si>
+    <t>T01A</t>
+  </si>
+  <si>
+    <t>DRG code</t>
+  </si>
+  <si>
+    <t>T01A/T01B</t>
+  </si>
+  <si>
+    <t>Average of T01A and T01B</t>
+  </si>
+  <si>
+    <t>T01B</t>
+  </si>
+  <si>
+    <t>T64B/T64C</t>
+  </si>
+  <si>
+    <t>Average of T64B and T64C</t>
+  </si>
+  <si>
+    <t>T64B</t>
+  </si>
+  <si>
+    <t>T64C</t>
   </si>
 </sst>
 </file>
@@ -1106,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1593,7 +1620,9 @@
       <c r="C38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="4"/>
+      <c r="D38" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
@@ -1605,6 +1634,9 @@
       <c r="C39" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D39" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
@@ -1616,6 +1648,9 @@
       <c r="C40" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="D40" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
@@ -1626,6 +1661,83 @@
       </c>
       <c r="C41" t="s">
         <v>70</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2">
+        <v>50828</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2">
+        <v>18592</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2">
+        <f>AVERAGE(A42:A43)</f>
+        <v>34710</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2">
+        <v>12233</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2">
+        <v>5199</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2">
+        <f>AVERAGE(A45:A46)</f>
+        <v>8716</v>
+      </c>
+      <c r="C47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cost Norovirus and non-STEC Ecoli
Also began to fix specialist visit assumptions (still to be finalised) and added total cost summaries to the shiny app
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831A39F8-5AD7-6847-A608-C95C1A053C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C9585-AFD9-B34B-8D4D-47B7D1CFE4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="460" windowWidth="18280" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="24440" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
   <si>
     <t>Cost</t>
   </si>
@@ -216,30 +216,15 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Cost in Ford2019 was not taken from MBS</t>
-  </si>
-  <si>
     <t>Stool_culture</t>
   </si>
   <si>
     <t>Ford2019</t>
   </si>
   <si>
-    <t>85% of benefit</t>
-  </si>
-  <si>
-    <t>85% of benefit for the sum of MBS codes 30473, 20902, 72818</t>
-  </si>
-  <si>
     <t>55832</t>
   </si>
   <si>
-    <t>85% of benefit - Ford2019 used code 55834 which is is cheaper in the current schedule but the cost difference depends on who refers rather than proceedure. The description for 55832 is lower leg ultrasound, however cost is the same for ultrasounds of knee, ankle etc.</t>
-  </si>
-  <si>
-    <t>85% of benefit !!!! Some oddities about how this is used. I have used this to lump together renal function test costs with ANA and EUC</t>
-  </si>
-  <si>
     <t>Weighted sum of MCS (69345) and PCR (69496). Following Ford2019 we used weights: 0.91 and .55. Weights don't add to 1 because 46% of people are thought to have both sets of tests</t>
   </si>
   <si>
@@ -271,6 +256,45 @@
   </si>
   <si>
     <t>T64C</t>
+  </si>
+  <si>
+    <t>benefit is 85% of fee</t>
+  </si>
+  <si>
+    <t>benefit is 85% of fee for the sum of MBS codes 30473, 20902, 72818</t>
+  </si>
+  <si>
+    <t>benefit is 85% of fee !!!! Also some oddities about how this is used. I have used this to lump together renal function test costs with ANA and EUC</t>
+  </si>
+  <si>
+    <t>benefit is 85% of fee - Ford2019 used code 55834 which is is cheaper in the current schedule but the cost difference depends on who refers rather than proceedure. The description for 55832 is lower leg ultrasound, however cost is the same for ultrasounds of knee, ankle etc.</t>
+  </si>
+  <si>
+    <t>TrimethoprimSulfamethoxazole</t>
+  </si>
+  <si>
+    <t>PBS general patient charge</t>
+  </si>
+  <si>
+    <t>10784N</t>
+  </si>
+  <si>
+    <t>physio</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>specialistRepeat</t>
+  </si>
+  <si>
+    <t>benefit is 85% of fee -- Cost in Ford2019 was not taken from MBS</t>
+  </si>
+  <si>
+    <t>specialist</t>
   </si>
 </sst>
 </file>
@@ -771,12 +795,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1133,15 +1158,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1182,562 +1209,617 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>315</v>
+        <v>67.8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>166</v>
+        <v>135.44999999999999</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>345.31</v>
+        <v>38.6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>11.36</v>
+        <v>76.8</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
+        <v>87</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>10.02</v>
+        <v>345.31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2">
-        <v>15.46</v>
+      <c r="A9" s="5">
+        <v>55.1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>10960</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>63</v>
+        <v>82</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>17.23</v>
+        <v>11.36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>11.6</v>
+        <v>10.02</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>72.650000000000006</v>
+        <v>15.46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>10.5</v>
+        <v>17.23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>8.99</v>
+        <v>11.6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>7.38</v>
+        <v>72.650000000000006</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>20.75</v>
+        <v>10.5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>87.65</v>
+        <v>8.99</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>3228.79</v>
+        <v>7.38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>76</v>
+        <v>20.75</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
+        <v>87.65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2">
+        <v>3228.79</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2">
+        <v>76</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2">
         <f xml:space="preserve"> 45 * 0.91 + 36.6 * 0.55</f>
         <v>61.080000000000005</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2">
-        <v>14.45</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2">
-        <v>6.7</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2">
-        <v>15.05</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>64</v>
-      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>9.6999999999999993</v>
+        <v>14.45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>21.05</v>
+        <v>6.7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>30.85</v>
+        <v>15.05</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>96.05</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
+        <v>21.05</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2">
+        <v>30.85</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2">
+        <v>96.05</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2">
         <f xml:space="preserve"> 155.3 + 69.4 + 91</f>
         <v>315.70000000000005</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="2">
-        <v>26.35</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="2">
-        <v>17.5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="2">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>9.65</v>
+        <v>26.35</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2">
-        <v>74.5</v>
+        <v>17.5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2">
-        <v>34.5</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2">
-        <v>66.45</v>
+        <v>9.65</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2">
-        <v>78.040000000000006</v>
+        <v>74.5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2">
-        <v>342.75</v>
+        <v>34.5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2">
-        <v>6155</v>
+        <v>66.45</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2">
-        <v>1961</v>
+        <v>78.040000000000006</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2">
-        <v>6364</v>
+        <v>342.75</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2">
-        <v>28927</v>
-      </c>
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" t="s">
-        <v>70</v>
+        <v>6155</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2">
-        <v>50828</v>
+        <v>1961</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
-        <v>18592</v>
+        <v>6364</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
-        <f>AVERAGE(A42:A43)</f>
-        <v>34710</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>73</v>
+        <v>28927</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2">
-        <v>12233</v>
+        <v>50828</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2">
-        <v>5199</v>
+        <v>18592</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
         <f>AVERAGE(A45:A46)</f>
+        <v>34710</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2">
+        <v>12233</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2">
+        <v>5199</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2">
+        <f>AVERAGE(A48:A49)</f>
         <v>8716</v>
       </c>
-      <c r="C47" t="s">
-        <v>76</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>77</v>
+      <c r="C50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2">
+        <v>35.97</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add in State surveillance diseases
STEC numbers are broken until we find the right Hospitalisation code
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946C9585-AFD9-B34B-8D4D-47B7D1CFE4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE003F8-0B26-5544-B368-25E66058AE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="24440" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
   <si>
     <t>Cost</t>
   </si>
@@ -294,7 +294,10 @@
     <t>benefit is 85% of fee -- Cost in Ford2019 was not taken from MBS</t>
   </si>
   <si>
-    <t>specialist</t>
+    <t>specialistInitial</t>
+  </si>
+  <si>
+    <t>L02B</t>
   </si>
 </sst>
 </file>
@@ -1158,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1822,6 +1825,20 @@
         <v>80</v>
       </c>
     </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2">
+        <v>6065</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated MBS scheme data
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlin/Repos_forked/FSANZ-ANU-Foodborne-Illness-Costing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE003F8-0B26-5544-B368-25E66058AE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397017D2-7AF6-1E4E-8953-1A5A7237AC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="24440" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="30200" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
   <si>
     <t>Cost</t>
   </si>
@@ -222,12 +222,6 @@
     <t>Ford2019</t>
   </si>
   <si>
-    <t>55832</t>
-  </si>
-  <si>
-    <t>Weighted sum of MCS (69345) and PCR (69496). Following Ford2019 we used weights: 0.91 and .55. Weights don't add to 1 because 46% of people are thought to have both sets of tests</t>
-  </si>
-  <si>
     <t>B06A</t>
   </si>
   <si>
@@ -261,15 +255,9 @@
     <t>benefit is 85% of fee</t>
   </si>
   <si>
-    <t>benefit is 85% of fee for the sum of MBS codes 30473, 20902, 72818</t>
-  </si>
-  <si>
     <t>benefit is 85% of fee !!!! Also some oddities about how this is used. I have used this to lump together renal function test costs with ANA and EUC</t>
   </si>
   <si>
-    <t>benefit is 85% of fee - Ford2019 used code 55834 which is is cheaper in the current schedule but the cost difference depends on who refers rather than proceedure. The description for 55832 is lower leg ultrasound, however cost is the same for ultrasounds of knee, ankle etc.</t>
-  </si>
-  <si>
     <t>TrimethoprimSulfamethoxazole</t>
   </si>
   <si>
@@ -298,6 +286,30 @@
   </si>
   <si>
     <t>L02B</t>
+  </si>
+  <si>
+    <t>55884</t>
+  </si>
+  <si>
+    <t>benefit is 85% of fee - Ford2019 used code 55834 which is is cheaper in the current schedule but the cost difference depends on who refers rather than proceedure. The description for 55832 is lower leg ultrasound, however cost is the same for ultrasounds of knee, ankle etc. Jan 2025 data update: MBS codes for single lower leg ultrasound (left or right) are 55884 and 55885 (depending on who refers). Values same for knee, ankle etc.</t>
+  </si>
+  <si>
+    <t>benefit is 85% of fee for the sum of MBS codes 30473 ($171.50), 20902 ($76.70), 72818 ($91.00)</t>
+  </si>
+  <si>
+    <t>Weighted sum of MCS 69345 ($45.00, 85% benefit) and PCR 69496 ($36.60, 85% benefit). Following Ford2019 we used weights: 0.91 and 0.55. Weights don't add to 1 because 46% of people are thought to have both sets of tests</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>MBS</t>
+  </si>
+  <si>
+    <t>DRG</t>
+  </si>
+  <si>
+    <t>PBS</t>
   </si>
 </sst>
 </file>
@@ -798,13 +810,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -865,9 +876,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -905,7 +916,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1011,7 +1022,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1153,7 +1164,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1161,20 +1172,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1184,13 +1196,16 @@
       <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>38.75</v>
+        <v>42.85</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1198,10 +1213,13 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
-        <v>75.05</v>
+        <v>122.15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1209,10 +1227,13 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
-        <v>67.8</v>
+        <v>74.25</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -1220,13 +1241,16 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
-        <v>135.44999999999999</v>
+        <v>148.35</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1234,204 +1258,230 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>38.6</v>
+        <v>42.3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>84.15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2">
-        <v>76.8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>345.31</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5">
-        <v>55.1</v>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>60.35</v>
       </c>
       <c r="B9" s="1">
         <v>10960</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>78</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>11.36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>10.02</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>15.46</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>17.23</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>11.6</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>72.650000000000006</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>10.5</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>8.99</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1"/>
+      <c r="E17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>7.38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1"/>
+      <c r="E18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>20.75</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1"/>
+      <c r="E19" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>87.65</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1"/>
+      <c r="E20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>3228.79</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
         <f xml:space="preserve"> 45 * 0.91 + 36.6 * 0.55</f>
         <v>61.080000000000005</v>
@@ -1439,13 +1489,14 @@
       <c r="C23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="D23" s="1"/>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>14.45</v>
       </c>
@@ -1455,11 +1506,14 @@
       <c r="C24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="D24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>6.7</v>
       </c>
@@ -1469,11 +1523,14 @@
       <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="D25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
         <v>15.05</v>
       </c>
@@ -1483,13 +1540,16 @@
       <c r="C26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="D26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
-        <v>9.6999999999999993</v>
+        <v>8.25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>30</v>
@@ -1497,11 +1557,14 @@
       <c r="C27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="D27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>21.05</v>
       </c>
@@ -1511,13 +1574,16 @@
       <c r="C28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="D28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
-        <v>30.85</v>
+        <v>34.1</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>34</v>
@@ -1525,13 +1591,16 @@
       <c r="C29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="D29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
-        <v>96.05</v>
+        <v>106</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -1539,23 +1608,28 @@
       <c r="C30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="D30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
-        <f xml:space="preserve"> 155.3 + 69.4 + 91</f>
-        <v>315.70000000000005</v>
+        <v>339.2</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="D31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
         <v>26.35</v>
       </c>
@@ -1565,11 +1639,14 @@
       <c r="C32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>17.5</v>
       </c>
@@ -1579,11 +1656,14 @@
       <c r="C33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>9.9499999999999993</v>
       </c>
@@ -1593,11 +1673,14 @@
       <c r="C34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>9.65</v>
       </c>
@@ -1607,13 +1690,16 @@
       <c r="C35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
-        <v>74.5</v>
+        <v>82.25</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>47</v>
@@ -1621,11 +1707,14 @@
       <c r="C36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>34.5</v>
       </c>
@@ -1635,13 +1724,16 @@
       <c r="C37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="D37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
-        <v>66.45</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>51</v>
@@ -1649,27 +1741,33 @@
       <c r="C38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
-        <v>78.040000000000006</v>
+        <v>104.05</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="D39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
-        <v>342.75</v>
+        <v>375.25</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>54</v>
@@ -1677,11 +1775,14 @@
       <c r="C40" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="D40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>6155</v>
       </c>
@@ -1691,11 +1792,14 @@
       <c r="C41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="D41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>1961</v>
       </c>
@@ -1705,11 +1809,14 @@
       <c r="C42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="D42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>6364</v>
       </c>
@@ -1719,127 +1826,160 @@
       <c r="C43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="D43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>28927</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C44" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>50828</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>64</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>18592</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>68</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="2">
         <f>AVERAGE(A45:A46)</f>
         <v>34710</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>66</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="2">
         <v>12233</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>71</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="2">
         <v>5199</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>72</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="2">
         <f>AVERAGE(A48:A49)</f>
         <v>8716</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>69</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="2">
         <v>35.97</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C51" t="s">
-        <v>79</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>75</v>
+      </c>
+      <c r="D51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="2">
         <v>6065</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>67</v>
+        <v>84</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="B32:B38 B24:B30 B39:B40 B2:B7" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update notes for costs to reflect new data.
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlin/Repos_forked/FSANZ-ANU-Foodborne-Illness-Costing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397017D2-7AF6-1E4E-8953-1A5A7237AC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ACFE56-01DD-6A4C-93E2-5D34DEF39CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="30200" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="93">
   <si>
     <t>Cost</t>
   </si>
@@ -252,12 +252,6 @@
     <t>T64C</t>
   </si>
   <si>
-    <t>benefit is 85% of fee</t>
-  </si>
-  <si>
-    <t>benefit is 85% of fee !!!! Also some oddities about how this is used. I have used this to lump together renal function test costs with ANA and EUC</t>
-  </si>
-  <si>
     <t>TrimethoprimSulfamethoxazole</t>
   </si>
   <si>
@@ -279,9 +273,6 @@
     <t>specialistRepeat</t>
   </si>
   <si>
-    <t>benefit is 85% of fee -- Cost in Ford2019 was not taken from MBS</t>
-  </si>
-  <si>
     <t>specialistInitial</t>
   </si>
   <si>
@@ -291,12 +282,6 @@
     <t>55884</t>
   </si>
   <si>
-    <t>benefit is 85% of fee - Ford2019 used code 55834 which is is cheaper in the current schedule but the cost difference depends on who refers rather than proceedure. The description for 55832 is lower leg ultrasound, however cost is the same for ultrasounds of knee, ankle etc. Jan 2025 data update: MBS codes for single lower leg ultrasound (left or right) are 55884 and 55885 (depending on who refers). Values same for knee, ankle etc.</t>
-  </si>
-  <si>
-    <t>benefit is 85% of fee for the sum of MBS codes 30473 ($171.50), 20902 ($76.70), 72818 ($91.00)</t>
-  </si>
-  <si>
     <t>Weighted sum of MCS 69345 ($45.00, 85% benefit) and PCR 69496 ($36.60, 85% benefit). Following Ford2019 we used weights: 0.91 and 0.55. Weights don't add to 1 because 46% of people are thought to have both sets of tests</t>
   </si>
   <si>
@@ -310,6 +295,21 @@
   </si>
   <si>
     <t>PBS</t>
+  </si>
+  <si>
+    <t>Emergency department admission - where does this number come from?</t>
+  </si>
+  <si>
+    <t>Benefit = 85% of fee</t>
+  </si>
+  <si>
+    <t>Benefit = 85% of fee for sum of MBS codes 30473 ($171.50), 20902 ($76.70), 72818 ($91.00)</t>
+  </si>
+  <si>
+    <t>Benefit = 85% of fee. MBS codes for single lower leg ultrasound (left or right) are 55884 and 55885 (depending on who refers). Values same for knee, ankle etc.</t>
+  </si>
+  <si>
+    <t>Benefit = 85% of fee. Note: some oddities about how this is used. I have used this to lump together renal function test costs with ANA and EUC</t>
   </si>
 </sst>
 </file>
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1197,7 +1197,7 @@
         <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
         <v>60</v>
@@ -1214,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1228,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1242,10 +1242,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1259,10 +1259,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1270,16 +1270,16 @@
         <v>42.3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1287,16 +1287,16 @@
         <v>84.15</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1307,6 +1307,9 @@
         <v>10</v>
       </c>
       <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2">
@@ -1316,13 +1319,13 @@
         <v>10960</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1489,9 +1492,11 @@
       <c r="C23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="2"/>
@@ -1507,10 +1512,10 @@
         <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1524,10 +1529,10 @@
         <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1541,10 +1546,10 @@
         <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1558,10 +1563,10 @@
         <v>31</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1575,10 +1580,10 @@
         <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1592,10 +1597,10 @@
         <v>35</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1609,10 +1614,10 @@
         <v>37</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1623,10 +1628,10 @@
         <v>38</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1640,10 +1645,10 @@
         <v>40</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E32" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1657,10 +1662,10 @@
         <v>42</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1674,10 +1679,10 @@
         <v>44</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1691,10 +1696,10 @@
         <v>46</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1708,10 +1713,10 @@
         <v>48</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1725,10 +1730,10 @@
         <v>50</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1742,10 +1747,10 @@
         <v>52</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1753,16 +1758,16 @@
         <v>104.05</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1776,10 +1781,10 @@
         <v>55</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="E40" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1793,7 +1798,7 @@
         <v>56</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>65</v>
@@ -1810,7 +1815,7 @@
         <v>57</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>65</v>
@@ -1827,7 +1832,7 @@
         <v>58</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>65</v>
@@ -1844,7 +1849,7 @@
         <v>63</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>65</v>
@@ -1861,7 +1866,7 @@
         <v>64</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>65</v>
@@ -1878,7 +1883,7 @@
         <v>68</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>65</v>
@@ -1893,7 +1898,7 @@
         <v>66</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>67</v>
@@ -1910,7 +1915,7 @@
         <v>71</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1924,7 +1929,7 @@
         <v>72</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1936,7 +1941,7 @@
         <v>69</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>70</v>
@@ -1947,16 +1952,16 @@
         <v>35.97</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1964,13 +1969,13 @@
         <v>6065</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Update DRG costs with NEP and weights
</commit_message>
<xml_diff>
--- a/Data/Costs.xlsx
+++ b/Data/Costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caitlin/Repos_forked/FSANZ-ANU-Foodborne-Illness-Costing/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E77BE0-CB0C-5645-A405-4C20C4280056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0620BC-FC2E-2147-92E2-5738500E868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="30200" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
   <si>
     <t>Cost</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t xml:space="preserve">pharmaceutical_costs.xslx </t>
+  </si>
+  <si>
+    <t>DRG code - price weight (inlier)</t>
   </si>
 </sst>
 </file>
@@ -813,13 +816,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1178,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1480,7 +1482,7 @@
       <c r="A22" s="2">
         <v>28.5</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22">
         <v>30087</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1798,7 +1800,8 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2">
-        <v>6155</v>
+        <f>5797*0.8276</f>
+        <v>4797.5972000000002</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>56</v>
@@ -1810,12 +1813,13 @@
         <v>84</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2">
-        <v>1961</v>
+        <f>5797*0.246</f>
+        <v>1426.0619999999999</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>57</v>
@@ -1827,12 +1831,13 @@
         <v>84</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2">
-        <v>6364</v>
+        <f>5797*0.2699</f>
+        <v>1564.6102999999998</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>58</v>
@@ -1844,12 +1849,13 @@
         <v>84</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2">
-        <v>28927</v>
+        <f>5797*7.3957</f>
+        <v>42872.872899999995</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>62</v>
@@ -1861,12 +1867,13 @@
         <v>84</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2">
-        <v>50828</v>
+        <f>5797*10.6081</f>
+        <v>61495.155700000003</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>63</v>
@@ -1878,12 +1885,13 @@
         <v>84</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2">
-        <v>18592</v>
+        <f xml:space="preserve"> 5797*5.3132</f>
+        <v>30800.6204</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>67</v>
@@ -1895,13 +1903,13 @@
         <v>84</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2">
         <f>AVERAGE(A45:A46)</f>
-        <v>34710</v>
+        <v>46147.888050000001</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>65</v>
@@ -1915,7 +1923,8 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2">
-        <v>12233</v>
+        <f>5797*2.2825</f>
+        <v>13231.652500000002</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>70</v>
@@ -1926,10 +1935,14 @@
       <c r="D48" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="E48" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2">
-        <v>5199</v>
+        <f>5797*1.224</f>
+        <v>7095.5280000000002</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>71</v>
@@ -1939,12 +1952,15 @@
       </c>
       <c r="D49" s="1" t="s">
         <v>84</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2">
         <f>AVERAGE(A48:A49)</f>
-        <v>8716</v>
+        <v>10163.590250000001</v>
       </c>
       <c r="C50" t="s">
         <v>68</v>

</xml_diff>